<commit_message>
progrès sur le cahier
</commit_message>
<xml_diff>
--- a/Docs/Fiche descriptive du Projet.xlsx
+++ b/Docs/Fiche descriptive du Projet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Fiche descriptive du projet tuteuré de S2</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Veronique Deslandres</t>
   </si>
   <si>
-    <t>Logiciels utilisable pour réaliser le projet</t>
-  </si>
-  <si>
     <t>Vrep(logiciel de simulation)</t>
   </si>
   <si>
@@ -71,12 +68,21 @@
   </si>
   <si>
     <t>Danguin Axel</t>
+  </si>
+  <si>
+    <t>OnShape (plans du robot)</t>
+  </si>
+  <si>
+    <t>Logiciels et matériel utilisables pour réaliser</t>
+  </si>
+  <si>
+    <t>le projet :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +123,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -252,61 +264,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,6 +432,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -435,6 +484,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C22"/>
+  <dimension ref="B1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,24 +690,24 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -654,100 +720,107 @@
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="23"/>
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="27"/>
+      <c r="C22" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28"/>
+      <c r="C23" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="C22" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B19:B22"/>
+  <mergeCells count="5">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B8:B11"/>
@@ -755,5 +828,6 @@
     <mergeCell ref="B12:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>